<commit_message>
replacing json fronmatter with yaml
</commit_message>
<xml_diff>
--- a/subtopic_indicator_groups.xlsx
+++ b/subtopic_indicator_groups.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G264"/>
+  <dimension ref="A1:H264"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -393,6 +393,11 @@
           <t>IndicatorID</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>order</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -426,6 +431,9 @@
       <c r="G2">
         <v>2390</v>
       </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -459,6 +467,9 @@
       <c r="G3">
         <v>2181</v>
       </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -492,6 +503,9 @@
       <c r="G4">
         <v>2158</v>
       </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -525,6 +539,9 @@
       <c r="G5">
         <v>2157</v>
       </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -558,6 +575,9 @@
       <c r="G6">
         <v>2389</v>
       </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -591,6 +611,9 @@
       <c r="G7">
         <v>2143</v>
       </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -624,6 +647,9 @@
       <c r="G8">
         <v>2388</v>
       </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -657,6 +683,9 @@
       <c r="G9">
         <v>2391</v>
       </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -690,6 +719,9 @@
       <c r="G10">
         <v>92</v>
       </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -723,6 +755,9 @@
       <c r="G11">
         <v>57</v>
       </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -756,6 +791,9 @@
       <c r="G12">
         <v>55</v>
       </c>
+      <c r="H12">
+        <v>11</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -789,6 +827,9 @@
       <c r="G13">
         <v>2024</v>
       </c>
+      <c r="H13">
+        <v>12</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -822,6 +863,9 @@
       <c r="G14">
         <v>2023</v>
       </c>
+      <c r="H14">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -855,6 +899,9 @@
       <c r="G15">
         <v>2028</v>
       </c>
+      <c r="H15">
+        <v>14</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -888,6 +935,9 @@
       <c r="G16">
         <v>2025</v>
       </c>
+      <c r="H16">
+        <v>15</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -921,6 +971,9 @@
       <c r="G17">
         <v>2027</v>
       </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -954,6 +1007,9 @@
       <c r="G18">
         <v>2026</v>
       </c>
+      <c r="H18">
+        <v>17</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -987,6 +1043,9 @@
       <c r="G19">
         <v>2049</v>
       </c>
+      <c r="H19">
+        <v>18</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1020,6 +1079,9 @@
       <c r="G20">
         <v>2057</v>
       </c>
+      <c r="H20">
+        <v>19</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1053,6 +1115,9 @@
       <c r="G21">
         <v>2050</v>
       </c>
+      <c r="H21">
+        <v>20</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1086,6 +1151,9 @@
       <c r="G22">
         <v>2051</v>
       </c>
+      <c r="H22">
+        <v>21</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1119,6 +1187,9 @@
       <c r="G23">
         <v>2056</v>
       </c>
+      <c r="H23">
+        <v>22</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1152,6 +1223,9 @@
       <c r="G24">
         <v>2055</v>
       </c>
+      <c r="H24">
+        <v>23</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1185,6 +1259,9 @@
       <c r="G25">
         <v>2380</v>
       </c>
+      <c r="H25">
+        <v>24</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1218,6 +1295,9 @@
       <c r="G26">
         <v>2384</v>
       </c>
+      <c r="H26">
+        <v>25</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1251,6 +1331,9 @@
       <c r="G27">
         <v>2048</v>
       </c>
+      <c r="H27">
+        <v>26</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1284,6 +1367,9 @@
       <c r="G28">
         <v>2378</v>
       </c>
+      <c r="H28">
+        <v>27</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1317,6 +1403,9 @@
       <c r="G29">
         <v>2379</v>
       </c>
+      <c r="H29">
+        <v>28</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1350,6 +1439,9 @@
       <c r="G30">
         <v>2383</v>
       </c>
+      <c r="H30">
+        <v>29</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1383,6 +1475,9 @@
       <c r="G31">
         <v>2382</v>
       </c>
+      <c r="H31">
+        <v>30</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1416,6 +1511,9 @@
       <c r="G32">
         <v>2387</v>
       </c>
+      <c r="H32">
+        <v>31</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1449,6 +1547,9 @@
       <c r="G33">
         <v>84</v>
       </c>
+      <c r="H33">
+        <v>32</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1482,6 +1583,9 @@
       <c r="G34">
         <v>2381</v>
       </c>
+      <c r="H34">
+        <v>33</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1515,6 +1619,9 @@
       <c r="G35">
         <v>2386</v>
       </c>
+      <c r="H35">
+        <v>34</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1548,6 +1655,9 @@
       <c r="G36">
         <v>18</v>
       </c>
+      <c r="H36">
+        <v>35</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1581,6 +1691,9 @@
       <c r="G37">
         <v>2392</v>
       </c>
+      <c r="H37">
+        <v>36</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1614,6 +1727,9 @@
       <c r="G38">
         <v>2147</v>
       </c>
+      <c r="H38">
+        <v>37</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1647,6 +1763,9 @@
       <c r="G39">
         <v>2149</v>
       </c>
+      <c r="H39">
+        <v>38</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1680,6 +1799,9 @@
       <c r="G40">
         <v>2339</v>
       </c>
+      <c r="H40">
+        <v>39</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1713,6 +1835,9 @@
       <c r="G41">
         <v>2030</v>
       </c>
+      <c r="H41">
+        <v>40</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1746,6 +1871,9 @@
       <c r="G42">
         <v>26</v>
       </c>
+      <c r="H42">
+        <v>41</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1779,6 +1907,9 @@
       <c r="G43">
         <v>30</v>
       </c>
+      <c r="H43">
+        <v>42</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1812,6 +1943,9 @@
       <c r="G44">
         <v>31</v>
       </c>
+      <c r="H44">
+        <v>43</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1845,6 +1979,9 @@
       <c r="G45">
         <v>36</v>
       </c>
+      <c r="H45">
+        <v>44</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1878,6 +2015,9 @@
       <c r="G46">
         <v>37</v>
       </c>
+      <c r="H46">
+        <v>45</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1911,6 +2051,9 @@
       <c r="G47">
         <v>33</v>
       </c>
+      <c r="H47">
+        <v>46</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1944,6 +2087,9 @@
       <c r="G48">
         <v>28</v>
       </c>
+      <c r="H48">
+        <v>47</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1977,6 +2123,9 @@
       <c r="G49">
         <v>32</v>
       </c>
+      <c r="H49">
+        <v>48</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2010,6 +2159,9 @@
       <c r="G50">
         <v>35</v>
       </c>
+      <c r="H50">
+        <v>49</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2043,6 +2195,9 @@
       <c r="G51">
         <v>27</v>
       </c>
+      <c r="H51">
+        <v>50</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2076,6 +2231,9 @@
       <c r="G52">
         <v>101</v>
       </c>
+      <c r="H52">
+        <v>51</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2109,6 +2267,9 @@
       <c r="G53">
         <v>29</v>
       </c>
+      <c r="H53">
+        <v>52</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2142,6 +2303,9 @@
       <c r="G54">
         <v>34</v>
       </c>
+      <c r="H54">
+        <v>53</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2175,6 +2339,9 @@
       <c r="G55">
         <v>5</v>
       </c>
+      <c r="H55">
+        <v>54</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2208,6 +2375,9 @@
       <c r="G56">
         <v>4</v>
       </c>
+      <c r="H56">
+        <v>55</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2241,6 +2411,9 @@
       <c r="G57">
         <v>6</v>
       </c>
+      <c r="H57">
+        <v>56</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2274,6 +2447,9 @@
       <c r="G58">
         <v>7</v>
       </c>
+      <c r="H58">
+        <v>57</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2307,6 +2483,9 @@
       <c r="G59">
         <v>8</v>
       </c>
+      <c r="H59">
+        <v>58</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2340,6 +2519,9 @@
       <c r="G60">
         <v>1</v>
       </c>
+      <c r="H60">
+        <v>59</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2373,6 +2555,9 @@
       <c r="G61">
         <v>10</v>
       </c>
+      <c r="H61">
+        <v>60</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2406,6 +2591,9 @@
       <c r="G62">
         <v>9</v>
       </c>
+      <c r="H62">
+        <v>61</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2439,6 +2627,9 @@
       <c r="G63">
         <v>3</v>
       </c>
+      <c r="H63">
+        <v>62</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2472,6 +2663,9 @@
       <c r="G64">
         <v>2</v>
       </c>
+      <c r="H64">
+        <v>63</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2505,6 +2699,9 @@
       <c r="G65">
         <v>74</v>
       </c>
+      <c r="H65">
+        <v>64</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2538,6 +2735,9 @@
       <c r="G66">
         <v>2096</v>
       </c>
+      <c r="H66">
+        <v>65</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2571,6 +2771,9 @@
       <c r="G67">
         <v>66</v>
       </c>
+      <c r="H67">
+        <v>66</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2604,6 +2807,9 @@
       <c r="G68">
         <v>60</v>
       </c>
+      <c r="H68">
+        <v>67</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2637,6 +2843,9 @@
       <c r="G69">
         <v>770</v>
       </c>
+      <c r="H69">
+        <v>68</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2670,6 +2879,9 @@
       <c r="G70">
         <v>2077</v>
       </c>
+      <c r="H70">
+        <v>69</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2703,6 +2915,9 @@
       <c r="G71">
         <v>2087</v>
       </c>
+      <c r="H71">
+        <v>70</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2736,6 +2951,9 @@
       <c r="G72">
         <v>2088</v>
       </c>
+      <c r="H72">
+        <v>71</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2769,6 +2987,9 @@
       <c r="G73">
         <v>73</v>
       </c>
+      <c r="H73">
+        <v>72</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2802,6 +3023,9 @@
       <c r="G74">
         <v>2089</v>
       </c>
+      <c r="H74">
+        <v>73</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2835,6 +3059,9 @@
       <c r="G75">
         <v>63</v>
       </c>
+      <c r="H75">
+        <v>74</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2868,6 +3095,9 @@
       <c r="G76">
         <v>2090</v>
       </c>
+      <c r="H76">
+        <v>75</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2901,6 +3131,9 @@
       <c r="G77">
         <v>2095</v>
       </c>
+      <c r="H77">
+        <v>76</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2934,6 +3167,9 @@
       <c r="G78">
         <v>71</v>
       </c>
+      <c r="H78">
+        <v>77</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2967,6 +3203,9 @@
       <c r="G79">
         <v>2091</v>
       </c>
+      <c r="H79">
+        <v>78</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3000,6 +3239,9 @@
       <c r="G80">
         <v>64</v>
       </c>
+      <c r="H80">
+        <v>79</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3033,6 +3275,9 @@
       <c r="G81">
         <v>690</v>
       </c>
+      <c r="H81">
+        <v>80</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3066,6 +3311,9 @@
       <c r="G82">
         <v>2037</v>
       </c>
+      <c r="H82">
+        <v>81</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3099,6 +3347,9 @@
       <c r="G83">
         <v>2035</v>
       </c>
+      <c r="H83">
+        <v>82</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3132,6 +3383,9 @@
       <c r="G84">
         <v>2033</v>
       </c>
+      <c r="H84">
+        <v>83</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3165,6 +3419,9 @@
       <c r="G85">
         <v>2031</v>
       </c>
+      <c r="H85">
+        <v>84</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3198,6 +3455,9 @@
       <c r="G86">
         <v>2039</v>
       </c>
+      <c r="H86">
+        <v>85</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3231,6 +3491,9 @@
       <c r="G87">
         <v>38</v>
       </c>
+      <c r="H87">
+        <v>86</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3264,6 +3527,9 @@
       <c r="G88">
         <v>2168</v>
       </c>
+      <c r="H88">
+        <v>87</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3297,6 +3563,9 @@
       <c r="G89">
         <v>2405</v>
       </c>
+      <c r="H89">
+        <v>88</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3330,6 +3599,9 @@
       <c r="G90">
         <v>2406</v>
       </c>
+      <c r="H90">
+        <v>89</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3363,6 +3635,9 @@
       <c r="G91">
         <v>2398</v>
       </c>
+      <c r="H91">
+        <v>90</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3396,6 +3671,9 @@
       <c r="G92">
         <v>2189</v>
       </c>
+      <c r="H92">
+        <v>91</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3429,6 +3707,9 @@
       <c r="G93">
         <v>2184</v>
       </c>
+      <c r="H93">
+        <v>92</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3462,6 +3743,9 @@
       <c r="G94">
         <v>2216</v>
       </c>
+      <c r="H94">
+        <v>93</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3495,6 +3779,9 @@
       <c r="G95">
         <v>2343</v>
       </c>
+      <c r="H95">
+        <v>94</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3528,6 +3815,9 @@
       <c r="G96">
         <v>2341</v>
       </c>
+      <c r="H96">
+        <v>95</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3561,6 +3851,9 @@
       <c r="G97">
         <v>2338</v>
       </c>
+      <c r="H97">
+        <v>96</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3594,6 +3887,9 @@
       <c r="G98">
         <v>2020</v>
       </c>
+      <c r="H98">
+        <v>97</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3627,6 +3923,9 @@
       <c r="G99">
         <v>2017</v>
       </c>
+      <c r="H99">
+        <v>98</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3660,6 +3959,9 @@
       <c r="G100">
         <v>2019</v>
       </c>
+      <c r="H100">
+        <v>99</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3693,6 +3995,9 @@
       <c r="G101">
         <v>2021</v>
       </c>
+      <c r="H101">
+        <v>100</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3726,6 +4031,9 @@
       <c r="G102">
         <v>25</v>
       </c>
+      <c r="H102">
+        <v>101</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3759,6 +4067,9 @@
       <c r="G103">
         <v>2141</v>
       </c>
+      <c r="H103">
+        <v>102</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3792,6 +4103,9 @@
       <c r="G104">
         <v>2143</v>
       </c>
+      <c r="H104">
+        <v>103</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3825,6 +4139,9 @@
       <c r="G105">
         <v>2084</v>
       </c>
+      <c r="H105">
+        <v>104</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3858,6 +4175,9 @@
       <c r="G106">
         <v>2191</v>
       </c>
+      <c r="H106">
+        <v>105</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3891,6 +4211,9 @@
       <c r="G107">
         <v>2411</v>
       </c>
+      <c r="H107">
+        <v>106</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3924,6 +4247,9 @@
       <c r="G108">
         <v>2155</v>
       </c>
+      <c r="H108">
+        <v>107</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3957,6 +4283,9 @@
       <c r="G109">
         <v>2104</v>
       </c>
+      <c r="H109">
+        <v>108</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3990,6 +4319,9 @@
       <c r="G110">
         <v>2185</v>
       </c>
+      <c r="H110">
+        <v>109</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4023,6 +4355,9 @@
       <c r="G111">
         <v>2377</v>
       </c>
+      <c r="H111">
+        <v>110</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4056,6 +4391,9 @@
       <c r="G112">
         <v>22</v>
       </c>
+      <c r="H112">
+        <v>111</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4089,6 +4427,9 @@
       <c r="G113">
         <v>2393</v>
       </c>
+      <c r="H113">
+        <v>112</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -4122,6 +4463,9 @@
       <c r="G114">
         <v>107</v>
       </c>
+      <c r="H114">
+        <v>113</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4155,6 +4499,9 @@
       <c r="G115">
         <v>2106</v>
       </c>
+      <c r="H115">
+        <v>114</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -4188,6 +4535,9 @@
       <c r="G116">
         <v>2207</v>
       </c>
+      <c r="H116">
+        <v>115</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -4221,6 +4571,9 @@
       <c r="G117">
         <v>2044</v>
       </c>
+      <c r="H117">
+        <v>116</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -4254,6 +4607,9 @@
       <c r="G118">
         <v>2043</v>
       </c>
+      <c r="H118">
+        <v>117</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -4287,6 +4643,9 @@
       <c r="G119">
         <v>2041</v>
       </c>
+      <c r="H119">
+        <v>118</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -4320,6 +4679,9 @@
       <c r="G120">
         <v>2135</v>
       </c>
+      <c r="H120">
+        <v>119</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -4353,6 +4715,9 @@
       <c r="G121">
         <v>2136</v>
       </c>
+      <c r="H121">
+        <v>120</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -4386,6 +4751,9 @@
       <c r="G122">
         <v>2408</v>
       </c>
+      <c r="H122">
+        <v>121</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -4419,6 +4787,9 @@
       <c r="G123">
         <v>2409</v>
       </c>
+      <c r="H123">
+        <v>122</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -4452,6 +4823,9 @@
       <c r="G124">
         <v>2403</v>
       </c>
+      <c r="H124">
+        <v>123</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -4485,6 +4859,9 @@
       <c r="G125">
         <v>2188</v>
       </c>
+      <c r="H125">
+        <v>124</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -4518,6 +4895,9 @@
       <c r="G126">
         <v>2151</v>
       </c>
+      <c r="H126">
+        <v>125</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -4551,6 +4931,9 @@
       <c r="G127">
         <v>2132</v>
       </c>
+      <c r="H127">
+        <v>126</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -4584,6 +4967,9 @@
       <c r="G128">
         <v>2401</v>
       </c>
+      <c r="H128">
+        <v>127</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -4617,6 +5003,9 @@
       <c r="G129">
         <v>2232</v>
       </c>
+      <c r="H129">
+        <v>128</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -4650,6 +5039,9 @@
       <c r="G130">
         <v>2122</v>
       </c>
+      <c r="H130">
+        <v>129</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -4683,6 +5075,9 @@
       <c r="G131">
         <v>2124</v>
       </c>
+      <c r="H131">
+        <v>130</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -4716,6 +5111,9 @@
       <c r="G132">
         <v>2121</v>
       </c>
+      <c r="H132">
+        <v>131</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -4749,6 +5147,9 @@
       <c r="G133">
         <v>2117</v>
       </c>
+      <c r="H133">
+        <v>132</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -4782,6 +5183,9 @@
       <c r="G134">
         <v>2120</v>
       </c>
+      <c r="H134">
+        <v>133</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -4815,6 +5219,9 @@
       <c r="G135">
         <v>2108</v>
       </c>
+      <c r="H135">
+        <v>134</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -4848,6 +5255,9 @@
       <c r="G136">
         <v>2119</v>
       </c>
+      <c r="H136">
+        <v>135</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -4881,6 +5291,9 @@
       <c r="G137">
         <v>2097</v>
       </c>
+      <c r="H137">
+        <v>136</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -4914,6 +5327,9 @@
       <c r="G138">
         <v>2389</v>
       </c>
+      <c r="H138">
+        <v>137</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -4947,6 +5363,9 @@
       <c r="G139">
         <v>2098</v>
       </c>
+      <c r="H139">
+        <v>138</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -4980,6 +5399,9 @@
       <c r="G140">
         <v>90</v>
       </c>
+      <c r="H140">
+        <v>139</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -5013,6 +5435,9 @@
       <c r="G141">
         <v>2101</v>
       </c>
+      <c r="H141">
+        <v>140</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -5046,6 +5471,9 @@
       <c r="G142">
         <v>25</v>
       </c>
+      <c r="H142">
+        <v>141</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -5079,6 +5507,9 @@
       <c r="G143">
         <v>2393</v>
       </c>
+      <c r="H143">
+        <v>142</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -5112,6 +5543,9 @@
       <c r="G144">
         <v>2394</v>
       </c>
+      <c r="H144">
+        <v>143</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -5145,6 +5579,9 @@
       <c r="G145">
         <v>107</v>
       </c>
+      <c r="H145">
+        <v>144</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -5178,6 +5615,9 @@
       <c r="G146">
         <v>48</v>
       </c>
+      <c r="H146">
+        <v>145</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -5211,6 +5651,9 @@
       <c r="G147">
         <v>2365</v>
       </c>
+      <c r="H147">
+        <v>146</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -5244,6 +5687,9 @@
       <c r="G148">
         <v>15</v>
       </c>
+      <c r="H148">
+        <v>147</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -5277,6 +5723,9 @@
       <c r="G149">
         <v>17</v>
       </c>
+      <c r="H149">
+        <v>148</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -5310,6 +5759,9 @@
       <c r="G150">
         <v>2396</v>
       </c>
+      <c r="H150">
+        <v>149</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -5343,6 +5795,9 @@
       <c r="G151">
         <v>2395</v>
       </c>
+      <c r="H151">
+        <v>150</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -5376,6 +5831,9 @@
       <c r="G152">
         <v>46</v>
       </c>
+      <c r="H152">
+        <v>151</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -5409,6 +5867,9 @@
       <c r="G153">
         <v>47</v>
       </c>
+      <c r="H153">
+        <v>152</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -5442,6 +5903,9 @@
       <c r="G154">
         <v>45</v>
       </c>
+      <c r="H154">
+        <v>153</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -5475,6 +5939,9 @@
       <c r="G155">
         <v>40</v>
       </c>
+      <c r="H155">
+        <v>154</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -5508,6 +5975,9 @@
       <c r="G156">
         <v>42</v>
       </c>
+      <c r="H156">
+        <v>155</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -5541,6 +6011,9 @@
       <c r="G157">
         <v>41</v>
       </c>
+      <c r="H157">
+        <v>156</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -5574,6 +6047,9 @@
       <c r="G158">
         <v>2399</v>
       </c>
+      <c r="H158">
+        <v>157</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -5607,6 +6083,9 @@
       <c r="G159">
         <v>2179</v>
       </c>
+      <c r="H159">
+        <v>158</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -5640,6 +6119,9 @@
       <c r="G160">
         <v>2188</v>
       </c>
+      <c r="H160">
+        <v>159</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -5673,6 +6155,9 @@
       <c r="G161">
         <v>2185</v>
       </c>
+      <c r="H161">
+        <v>160</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -5706,6 +6191,9 @@
       <c r="G162">
         <v>2377</v>
       </c>
+      <c r="H162">
+        <v>161</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -5739,6 +6227,9 @@
       <c r="G163">
         <v>2176</v>
       </c>
+      <c r="H163">
+        <v>162</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -5772,6 +6263,9 @@
       <c r="G164">
         <v>16</v>
       </c>
+      <c r="H164">
+        <v>163</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -5805,6 +6299,9 @@
       <c r="G165">
         <v>41</v>
       </c>
+      <c r="H165">
+        <v>164</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -5838,6 +6335,9 @@
       <c r="G166">
         <v>2105</v>
       </c>
+      <c r="H166">
+        <v>165</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -5871,6 +6371,9 @@
       <c r="G167">
         <v>24</v>
       </c>
+      <c r="H167">
+        <v>166</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -5904,6 +6407,9 @@
       <c r="G168">
         <v>2394</v>
       </c>
+      <c r="H168">
+        <v>167</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -5937,6 +6443,9 @@
       <c r="G169">
         <v>48</v>
       </c>
+      <c r="H169">
+        <v>168</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -5970,6 +6479,9 @@
       <c r="G170">
         <v>5</v>
       </c>
+      <c r="H170">
+        <v>169</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -6003,6 +6515,9 @@
       <c r="G171">
         <v>6</v>
       </c>
+      <c r="H171">
+        <v>170</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -6036,6 +6551,9 @@
       <c r="G172">
         <v>8</v>
       </c>
+      <c r="H172">
+        <v>171</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -6069,6 +6587,9 @@
       <c r="G173">
         <v>2322</v>
       </c>
+      <c r="H173">
+        <v>172</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -6102,6 +6623,9 @@
       <c r="G174">
         <v>2043</v>
       </c>
+      <c r="H174">
+        <v>173</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -6135,6 +6659,9 @@
       <c r="G175">
         <v>2146</v>
       </c>
+      <c r="H175">
+        <v>174</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -6168,6 +6695,9 @@
       <c r="G176">
         <v>2325</v>
       </c>
+      <c r="H176">
+        <v>175</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -6201,6 +6731,9 @@
       <c r="G177">
         <v>2112</v>
       </c>
+      <c r="H177">
+        <v>176</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -6234,6 +6767,9 @@
       <c r="G178">
         <v>2114</v>
       </c>
+      <c r="H178">
+        <v>177</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -6267,6 +6803,9 @@
       <c r="G179">
         <v>2157</v>
       </c>
+      <c r="H179">
+        <v>178</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -6300,6 +6839,9 @@
       <c r="G180">
         <v>2133</v>
       </c>
+      <c r="H180">
+        <v>179</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -6333,6 +6875,9 @@
       <c r="G181">
         <v>2414</v>
       </c>
+      <c r="H181">
+        <v>180</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -6366,6 +6911,9 @@
       <c r="G182">
         <v>2063</v>
       </c>
+      <c r="H182">
+        <v>181</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -6399,6 +6947,9 @@
       <c r="G183">
         <v>2064</v>
       </c>
+      <c r="H183">
+        <v>182</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -6432,6 +6983,9 @@
       <c r="G184">
         <v>2061</v>
       </c>
+      <c r="H184">
+        <v>183</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -6465,6 +7019,9 @@
       <c r="G185">
         <v>2062</v>
       </c>
+      <c r="H185">
+        <v>184</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -6498,6 +7055,9 @@
       <c r="G186">
         <v>2235</v>
       </c>
+      <c r="H186">
+        <v>185</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -6531,6 +7091,9 @@
       <c r="G187">
         <v>91</v>
       </c>
+      <c r="H187">
+        <v>186</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -6564,6 +7127,9 @@
       <c r="G188">
         <v>100</v>
       </c>
+      <c r="H188">
+        <v>187</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -6597,6 +7163,9 @@
       <c r="G189">
         <v>2312</v>
       </c>
+      <c r="H189">
+        <v>188</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -6630,6 +7199,9 @@
       <c r="G190">
         <v>96</v>
       </c>
+      <c r="H190">
+        <v>189</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -6663,6 +7235,9 @@
       <c r="G191">
         <v>94</v>
       </c>
+      <c r="H191">
+        <v>190</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -6696,6 +7271,9 @@
       <c r="G192">
         <v>93</v>
       </c>
+      <c r="H192">
+        <v>191</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -6729,6 +7307,9 @@
       <c r="G193">
         <v>99</v>
       </c>
+      <c r="H193">
+        <v>192</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -6762,6 +7343,9 @@
       <c r="G194">
         <v>97</v>
       </c>
+      <c r="H194">
+        <v>193</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -6795,6 +7379,9 @@
       <c r="G195">
         <v>98</v>
       </c>
+      <c r="H195">
+        <v>194</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -6828,6 +7415,9 @@
       <c r="G196">
         <v>102</v>
       </c>
+      <c r="H196">
+        <v>195</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -6861,6 +7451,9 @@
       <c r="G197">
         <v>2366</v>
       </c>
+      <c r="H197">
+        <v>196</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -6894,6 +7487,9 @@
       <c r="G198">
         <v>2364</v>
       </c>
+      <c r="H198">
+        <v>197</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -6927,6 +7523,9 @@
       <c r="G199">
         <v>2367</v>
       </c>
+      <c r="H199">
+        <v>198</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -6960,6 +7559,9 @@
       <c r="G200">
         <v>2368</v>
       </c>
+      <c r="H200">
+        <v>199</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -6993,6 +7595,9 @@
       <c r="G201">
         <v>2369</v>
       </c>
+      <c r="H201">
+        <v>200</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -7026,6 +7631,9 @@
       <c r="G202">
         <v>2374</v>
       </c>
+      <c r="H202">
+        <v>201</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -7059,6 +7667,9 @@
       <c r="G203">
         <v>2370</v>
       </c>
+      <c r="H203">
+        <v>202</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -7092,6 +7703,9 @@
       <c r="G204">
         <v>2060</v>
       </c>
+      <c r="H204">
+        <v>203</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -7125,6 +7739,9 @@
       <c r="G205">
         <v>2058</v>
       </c>
+      <c r="H205">
+        <v>204</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -7158,6 +7775,9 @@
       <c r="G206">
         <v>2173</v>
       </c>
+      <c r="H206">
+        <v>205</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -7191,6 +7811,9 @@
       <c r="G207">
         <v>2059</v>
       </c>
+      <c r="H207">
+        <v>206</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -7224,6 +7847,9 @@
       <c r="G208">
         <v>2172</v>
       </c>
+      <c r="H208">
+        <v>207</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -7257,6 +7883,9 @@
       <c r="G209">
         <v>2065</v>
       </c>
+      <c r="H209">
+        <v>208</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -7290,6 +7919,9 @@
       <c r="G210">
         <v>2145</v>
       </c>
+      <c r="H210">
+        <v>209</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -7323,6 +7955,9 @@
       <c r="G211">
         <v>2176</v>
       </c>
+      <c r="H211">
+        <v>210</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -7356,6 +7991,9 @@
       <c r="G212">
         <v>14</v>
       </c>
+      <c r="H212">
+        <v>211</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -7389,6 +8027,9 @@
       <c r="G213">
         <v>2334</v>
       </c>
+      <c r="H213">
+        <v>212</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -7422,6 +8063,9 @@
       <c r="G214">
         <v>2317</v>
       </c>
+      <c r="H214">
+        <v>213</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -7455,6 +8099,9 @@
       <c r="G215">
         <v>2335</v>
       </c>
+      <c r="H215">
+        <v>214</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -7488,6 +8135,9 @@
       <c r="G216">
         <v>2146</v>
       </c>
+      <c r="H216">
+        <v>215</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -7521,6 +8171,9 @@
       <c r="G217">
         <v>2073</v>
       </c>
+      <c r="H217">
+        <v>216</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -7554,6 +8207,9 @@
       <c r="G218">
         <v>103</v>
       </c>
+      <c r="H218">
+        <v>217</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -7587,6 +8243,9 @@
       <c r="G219">
         <v>2325</v>
       </c>
+      <c r="H219">
+        <v>218</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -7620,6 +8279,9 @@
       <c r="G220">
         <v>2336</v>
       </c>
+      <c r="H220">
+        <v>219</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -7653,6 +8315,9 @@
       <c r="G221">
         <v>2323</v>
       </c>
+      <c r="H221">
+        <v>220</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -7686,6 +8351,9 @@
       <c r="G222">
         <v>2337</v>
       </c>
+      <c r="H222">
+        <v>221</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -7719,6 +8387,9 @@
       <c r="G223">
         <v>2389</v>
       </c>
+      <c r="H223">
+        <v>222</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -7752,6 +8423,9 @@
       <c r="G224">
         <v>2365</v>
       </c>
+      <c r="H224">
+        <v>223</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -7785,6 +8459,9 @@
       <c r="G225">
         <v>15</v>
       </c>
+      <c r="H225">
+        <v>224</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -7818,6 +8495,9 @@
       <c r="G226">
         <v>17</v>
       </c>
+      <c r="H226">
+        <v>225</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -7851,6 +8531,9 @@
       <c r="G227">
         <v>2097</v>
       </c>
+      <c r="H227">
+        <v>226</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -7884,6 +8567,9 @@
       <c r="G228">
         <v>2098</v>
       </c>
+      <c r="H228">
+        <v>227</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -7917,6 +8603,9 @@
       <c r="G229">
         <v>2236</v>
       </c>
+      <c r="H229">
+        <v>228</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -7950,6 +8639,9 @@
       <c r="G230">
         <v>2112</v>
       </c>
+      <c r="H230">
+        <v>229</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -7983,6 +8675,9 @@
       <c r="G231">
         <v>2113</v>
       </c>
+      <c r="H231">
+        <v>230</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -8016,6 +8711,9 @@
       <c r="G232">
         <v>2114</v>
       </c>
+      <c r="H232">
+        <v>231</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -8049,6 +8747,9 @@
       <c r="G233">
         <v>2092</v>
       </c>
+      <c r="H233">
+        <v>232</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -8082,6 +8783,9 @@
       <c r="G234">
         <v>2086</v>
       </c>
+      <c r="H234">
+        <v>233</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -8115,6 +8819,9 @@
       <c r="G235">
         <v>2094</v>
       </c>
+      <c r="H235">
+        <v>234</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -8148,6 +8855,9 @@
       <c r="G236">
         <v>2093</v>
       </c>
+      <c r="H236">
+        <v>235</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -8181,6 +8891,9 @@
       <c r="G237">
         <v>2218</v>
       </c>
+      <c r="H237">
+        <v>236</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -8214,6 +8927,9 @@
       <c r="G238">
         <v>2340</v>
       </c>
+      <c r="H238">
+        <v>237</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -8247,6 +8963,9 @@
       <c r="G239">
         <v>2400</v>
       </c>
+      <c r="H239">
+        <v>238</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -8280,6 +8999,9 @@
       <c r="G240">
         <v>2375</v>
       </c>
+      <c r="H240">
+        <v>239</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -8313,6 +9035,9 @@
       <c r="G241">
         <v>2236</v>
       </c>
+      <c r="H241">
+        <v>240</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -8346,6 +9071,9 @@
       <c r="G242">
         <v>2237</v>
       </c>
+      <c r="H242">
+        <v>241</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -8379,6 +9107,9 @@
       <c r="G243">
         <v>2238</v>
       </c>
+      <c r="H243">
+        <v>242</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -8412,6 +9143,9 @@
       <c r="G244">
         <v>2058</v>
       </c>
+      <c r="H244">
+        <v>243</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -8445,6 +9179,9 @@
       <c r="G245">
         <v>2173</v>
       </c>
+      <c r="H245">
+        <v>244</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -8478,6 +9215,9 @@
       <c r="G246">
         <v>2059</v>
       </c>
+      <c r="H246">
+        <v>245</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -8511,6 +9251,9 @@
       <c r="G247">
         <v>2172</v>
       </c>
+      <c r="H247">
+        <v>246</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -8544,6 +9287,9 @@
       <c r="G248">
         <v>2376</v>
       </c>
+      <c r="H248">
+        <v>247</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -8577,6 +9323,9 @@
       <c r="G249">
         <v>2175</v>
       </c>
+      <c r="H249">
+        <v>248</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -8610,6 +9359,9 @@
       <c r="G250">
         <v>2174</v>
       </c>
+      <c r="H250">
+        <v>249</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -8643,6 +9395,9 @@
       <c r="G251">
         <v>2410</v>
       </c>
+      <c r="H251">
+        <v>250</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -8676,6 +9431,9 @@
       <c r="G252">
         <v>2084</v>
       </c>
+      <c r="H252">
+        <v>251</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -8709,6 +9467,9 @@
       <c r="G253">
         <v>2074</v>
       </c>
+      <c r="H253">
+        <v>252</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -8742,6 +9503,9 @@
       <c r="G254">
         <v>2075</v>
       </c>
+      <c r="H254">
+        <v>253</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -8775,6 +9539,9 @@
       <c r="G255">
         <v>2076</v>
       </c>
+      <c r="H255">
+        <v>254</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -8808,6 +9575,9 @@
       <c r="G256">
         <v>2191</v>
       </c>
+      <c r="H256">
+        <v>255</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -8841,6 +9611,9 @@
       <c r="G257">
         <v>2411</v>
       </c>
+      <c r="H257">
+        <v>256</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -8874,6 +9647,9 @@
       <c r="G258">
         <v>2209</v>
       </c>
+      <c r="H258">
+        <v>257</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -8907,6 +9683,9 @@
       <c r="G259">
         <v>2211</v>
       </c>
+      <c r="H259">
+        <v>258</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -8940,6 +9719,9 @@
       <c r="G260">
         <v>2208</v>
       </c>
+      <c r="H260">
+        <v>259</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -8973,6 +9755,9 @@
       <c r="G261">
         <v>2210</v>
       </c>
+      <c r="H261">
+        <v>260</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -9006,6 +9791,9 @@
       <c r="G262">
         <v>2214</v>
       </c>
+      <c r="H262">
+        <v>261</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -9039,6 +9827,9 @@
       <c r="G263">
         <v>2239</v>
       </c>
+      <c r="H263">
+        <v>262</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -9071,6 +9862,9 @@
       </c>
       <c r="G264">
         <v>2215</v>
+      </c>
+      <c r="H264">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>